<commit_message>
Corrected Equipment List to match source code and Kilroy
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2017.xlsx
+++ b/Kilroy Equipment List 2017.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robotics\2017\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10596" windowHeight="5796"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -201,12 +196,6 @@
     <t>PWM 3</t>
   </si>
   <si>
-    <t>3, 4</t>
-  </si>
-  <si>
-    <t>5, 6</t>
-  </si>
-  <si>
     <t>Kilroy Equipment List (2017)</t>
   </si>
   <si>
@@ -214,13 +203,19 @@
   </si>
   <si>
     <t xml:space="preserve">Left Rear Motor Controller </t>
+  </si>
+  <si>
+    <t>10, 11</t>
+  </si>
+  <si>
+    <t>12, 13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -948,37 +943,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F101" sqref="F101"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="55" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="55" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" style="55" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="55" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="55" customWidth="1"/>
     <col min="4" max="4" width="21" style="56" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" style="58" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="55" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="55"/>
-    <col min="8" max="8" width="11.109375" style="55" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="55"/>
+    <col min="5" max="5" width="18.140625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="55" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="55"/>
+    <col min="8" max="8" width="11.140625" style="55" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="68" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
       <c r="D1" s="68"/>
       <c r="E1" s="68"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -995,7 +990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="67" t="s">
@@ -1006,11 +1001,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>37</v>
@@ -1019,11 +1014,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="60"/>
       <c r="B5" s="60"/>
       <c r="C5" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>38</v>
@@ -1032,21 +1027,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
     </row>
-    <row r="7" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="34" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="28"/>
       <c r="D7" s="31"/>
       <c r="E7" s="32"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="48"/>
@@ -1056,7 +1051,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="66"/>
@@ -1066,7 +1061,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25"/>
@@ -1076,21 +1071,21 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="1" customFormat="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="1" customFormat="1">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="69" t="s">
@@ -1101,21 +1096,21 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="1" customFormat="1">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="28"/>
       <c r="D14" s="31"/>
       <c r="E14" s="32"/>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="1" customFormat="1">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="25"/>
       <c r="D15" s="26"/>
       <c r="E15" s="43"/>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="1" customFormat="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="28"/>
@@ -1125,7 +1120,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="1" customFormat="1">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="25"/>
@@ -1135,7 +1130,7 @@
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="1" customFormat="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="5"/>
@@ -1145,7 +1140,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="1" customFormat="1">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
@@ -1155,7 +1150,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="1" customFormat="1">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1165,7 +1160,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="1" customFormat="1">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -1175,7 +1170,7 @@
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="1" customFormat="1">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -1185,7 +1180,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="1" customFormat="1">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
@@ -1195,21 +1190,21 @@
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="1" customFormat="1">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="1" customFormat="1">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="67" t="s">
@@ -1220,7 +1215,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="1" customFormat="1">
       <c r="A27" s="42"/>
       <c r="B27" s="42"/>
       <c r="C27" s="28" t="s">
@@ -1230,10 +1225,10 @@
         <v>39</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="1" customFormat="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="22" t="s">
@@ -1243,108 +1238,108 @@
         <v>41</v>
       </c>
       <c r="E28" s="43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="1" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="28"/>
       <c r="D29" s="31"/>
       <c r="E29" s="32"/>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="22"/>
       <c r="D30" s="44"/>
       <c r="E30" s="43"/>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="28"/>
       <c r="D31" s="31"/>
       <c r="E31" s="32"/>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="22"/>
       <c r="D32" s="44"/>
       <c r="E32" s="43"/>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="1" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="28"/>
       <c r="D33" s="31"/>
       <c r="E33" s="32"/>
     </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="22"/>
       <c r="D34" s="44"/>
       <c r="E34" s="43"/>
     </row>
-    <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="62"/>
       <c r="D35" s="63"/>
       <c r="E35" s="64"/>
     </row>
-    <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="1" customFormat="1">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="25"/>
       <c r="D36" s="65"/>
       <c r="E36" s="52"/>
     </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="28"/>
       <c r="D37" s="31"/>
       <c r="E37" s="32"/>
     </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="22"/>
       <c r="D38" s="44"/>
       <c r="E38" s="43"/>
     </row>
-    <row r="39" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="53"/>
       <c r="D39" s="31"/>
       <c r="E39" s="32"/>
     </row>
-    <row r="40" spans="1:5" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" s="18" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="22"/>
       <c r="D42" s="44"/>
       <c r="E42" s="43"/>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="67" t="s">
@@ -1355,7 +1350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="1" customFormat="1">
       <c r="A44" s="39" t="s">
         <v>6</v>
       </c>
@@ -1366,14 +1361,14 @@
       <c r="D44" s="24"/>
       <c r="E44" s="46"/>
     </row>
-    <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="1" customFormat="1">
       <c r="A45" s="40"/>
       <c r="B45" s="14"/>
       <c r="C45" s="41"/>
       <c r="D45" s="44"/>
       <c r="E45" s="14"/>
     </row>
-    <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="1" customFormat="1">
       <c r="A46" s="4" t="s">
         <v>6</v>
       </c>
@@ -1384,14 +1379,14 @@
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="1" customFormat="1">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
       <c r="E47" s="11"/>
     </row>
-    <row r="48" spans="1:5" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="67" t="s">
@@ -1402,49 +1397,49 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="18" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="45"/>
       <c r="D49" s="24"/>
       <c r="E49" s="46"/>
     </row>
-    <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" s="1" customFormat="1">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="25"/>
       <c r="D50" s="26"/>
       <c r="E50" s="27"/>
     </row>
-    <row r="51" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" s="1" customFormat="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="28"/>
       <c r="D51" s="31"/>
       <c r="E51" s="32"/>
     </row>
-    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="1" customFormat="1">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="25"/>
       <c r="D52" s="26"/>
       <c r="E52" s="27"/>
     </row>
-    <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" s="1" customFormat="1">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="28"/>
       <c r="D53" s="31"/>
       <c r="E53" s="32"/>
     </row>
-    <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="1" customFormat="1">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="25"/>
       <c r="D54" s="26"/>
       <c r="E54" s="27"/>
     </row>
-    <row r="55" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
       <c r="C55" s="67" t="s">
@@ -1455,35 +1450,35 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" s="1" customFormat="1">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="45"/>
       <c r="D56" s="24"/>
       <c r="E56" s="32"/>
     </row>
-    <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" s="1" customFormat="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="25"/>
       <c r="D57" s="26"/>
       <c r="E57" s="27"/>
     </row>
-    <row r="58" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" s="1" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="28"/>
       <c r="D58" s="31"/>
       <c r="E58" s="32"/>
     </row>
-    <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" s="1" customFormat="1">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="25"/>
       <c r="D59" s="26"/>
       <c r="E59" s="27"/>
     </row>
-    <row r="60" spans="1:8" s="35" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
@@ -1492,7 +1487,7 @@
       <c r="G60" s="36"/>
       <c r="H60" s="36"/>
     </row>
-    <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="67" t="s">
@@ -1503,28 +1498,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="1" customFormat="1">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
       <c r="E62" s="11"/>
     </row>
-    <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" s="1" customFormat="1">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="5"/>
       <c r="D63" s="6"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" s="1" customFormat="1">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="11"/>
     </row>
-    <row r="65" spans="1:8" s="35" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
@@ -1533,7 +1528,7 @@
       <c r="G65" s="36"/>
       <c r="H65" s="36"/>
     </row>
-    <row r="66" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="67" t="s">
@@ -1545,7 +1540,7 @@
       </c>
       <c r="G66" s="20"/>
     </row>
-    <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" s="1" customFormat="1">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="25" t="s">
@@ -1559,7 +1554,7 @@
       </c>
       <c r="G67" s="20"/>
     </row>
-    <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" s="1" customFormat="1">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="28" t="s">
@@ -1573,7 +1568,7 @@
       </c>
       <c r="G68" s="20"/>
     </row>
-    <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" s="1" customFormat="1">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="22" t="s">
@@ -1587,7 +1582,7 @@
       </c>
       <c r="G69" s="20"/>
     </row>
-    <row r="70" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" s="1" customFormat="1">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="28" t="s">
@@ -1601,7 +1596,7 @@
       </c>
       <c r="G70" s="20"/>
     </row>
-    <row r="71" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="67" t="s">
@@ -1613,49 +1608,49 @@
       </c>
       <c r="G71" s="20"/>
     </row>
-    <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" s="1" customFormat="1">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="23"/>
       <c r="D72" s="26"/>
       <c r="E72" s="25"/>
     </row>
-    <row r="73" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" s="35" customFormat="1">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="28"/>
       <c r="D73" s="31"/>
       <c r="E73" s="32"/>
     </row>
-    <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" s="1" customFormat="1">
       <c r="A74" s="47"/>
       <c r="B74" s="47"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
     </row>
-    <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" s="1" customFormat="1">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="32"/>
       <c r="D75" s="31"/>
       <c r="E75" s="32"/>
     </row>
-    <row r="76" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" s="1" customFormat="1">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="25"/>
       <c r="D76" s="10"/>
       <c r="E76" s="27"/>
     </row>
-    <row r="77" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" s="1" customFormat="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="28"/>
       <c r="D77" s="31"/>
       <c r="E77" s="32"/>
     </row>
-    <row r="78" spans="1:8" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="8"/>
       <c r="C78" s="29"/>
@@ -1663,14 +1658,14 @@
       <c r="E78" s="43"/>
       <c r="F78" s="20"/>
     </row>
-    <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" s="1" customFormat="1">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="28"/>
       <c r="D79" s="31"/>
       <c r="E79" s="32"/>
     </row>
-    <row r="80" spans="1:8" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="8"/>
       <c r="C80" s="22"/>
@@ -1678,14 +1673,14 @@
       <c r="E80" s="43"/>
       <c r="F80" s="20"/>
     </row>
-    <row r="81" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="1" customFormat="1">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="28"/>
       <c r="D81" s="31"/>
       <c r="E81" s="32"/>
     </row>
-    <row r="82" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A82" s="13"/>
       <c r="B82" s="8"/>
       <c r="C82" s="22"/>
@@ -1693,14 +1688,14 @@
       <c r="E82" s="23"/>
       <c r="F82" s="20"/>
     </row>
-    <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="1" customFormat="1">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="28"/>
       <c r="D83" s="31"/>
       <c r="E83" s="32"/>
     </row>
-    <row r="84" spans="1:7" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A84" s="13"/>
       <c r="B84" s="8"/>
       <c r="C84" s="22"/>
@@ -1708,14 +1703,14 @@
       <c r="E84" s="43"/>
       <c r="F84" s="20"/>
     </row>
-    <row r="85" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" s="1" customFormat="1">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="28"/>
       <c r="D85" s="6"/>
       <c r="E85" s="32"/>
     </row>
-    <row r="86" spans="1:7" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A86" s="13"/>
       <c r="B86" s="8"/>
       <c r="C86" s="22"/>
@@ -1723,14 +1718,14 @@
       <c r="E86" s="43"/>
       <c r="F86" s="20"/>
     </row>
-    <row r="87" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" s="1" customFormat="1">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="28"/>
       <c r="D87" s="31"/>
       <c r="E87" s="32"/>
     </row>
-    <row r="88" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A88" s="13"/>
       <c r="B88" s="8"/>
       <c r="C88" s="22"/>
@@ -1738,14 +1733,14 @@
       <c r="E88" s="43"/>
       <c r="F88" s="20"/>
     </row>
-    <row r="89" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="28"/>
       <c r="D89" s="31"/>
       <c r="E89" s="32"/>
     </row>
-    <row r="90" spans="1:7" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A90" s="13"/>
       <c r="B90" s="8"/>
       <c r="C90" s="22"/>
@@ -1753,14 +1748,14 @@
       <c r="E90" s="43"/>
       <c r="F90" s="20"/>
     </row>
-    <row r="91" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" s="1" customFormat="1">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="28"/>
       <c r="D91" s="31"/>
       <c r="E91" s="32"/>
     </row>
-    <row r="92" spans="1:7" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
       <c r="C92" s="67" t="s">
@@ -1772,7 +1767,7 @@
       </c>
       <c r="G92" s="20"/>
     </row>
-    <row r="93" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" s="1" customFormat="1">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="23" t="s">
@@ -1785,49 +1780,49 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" s="1" customFormat="1">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="5"/>
       <c r="D94" s="6"/>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="1" customFormat="1">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="22"/>
       <c r="D95" s="15"/>
       <c r="E95" s="16"/>
     </row>
-    <row r="96" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="1" customFormat="1">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="5"/>
       <c r="D96" s="6"/>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:6" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="20"/>
       <c r="D97" s="15"/>
       <c r="E97" s="16"/>
     </row>
-    <row r="98" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" s="1" customFormat="1">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="5"/>
       <c r="D98" s="6"/>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" s="1" customFormat="1">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:6" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="5"/>
@@ -1835,21 +1830,21 @@
       <c r="E100" s="7"/>
       <c r="F100" s="20"/>
     </row>
-    <row r="101" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" s="1" customFormat="1">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="14"/>
       <c r="D101" s="15"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" s="1" customFormat="1">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="5"/>
       <c r="D102" s="6"/>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" s="1" customFormat="1">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
       <c r="C103" s="54" t="s">
@@ -1860,7 +1855,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" s="1" customFormat="1">
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="C104" s="9" t="s">
@@ -1873,7 +1868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" s="1" customFormat="1">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="5" t="s">
@@ -1886,7 +1881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" s="1" customFormat="1">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="25" t="s">
@@ -1899,7 +1894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" s="1" customFormat="1">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="28" t="s">
@@ -1912,7 +1907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" s="1" customFormat="1">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="C108" s="22" t="s">
@@ -1925,910 +1920,910 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" s="1" customFormat="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="28"/>
       <c r="D109" s="6"/>
       <c r="E109" s="32"/>
     </row>
-    <row r="110" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" s="1" customFormat="1">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="C110" s="22"/>
       <c r="D110" s="44"/>
       <c r="E110" s="22"/>
     </row>
-    <row r="111" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" s="1" customFormat="1">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="28"/>
       <c r="D111" s="6"/>
       <c r="E111" s="32"/>
     </row>
-    <row r="112" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" s="1" customFormat="1">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="22"/>
       <c r="D112" s="44"/>
       <c r="E112" s="22"/>
     </row>
-    <row r="113" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" s="1" customFormat="1">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="28"/>
       <c r="D113" s="31"/>
       <c r="E113" s="32"/>
     </row>
-    <row r="114" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" s="1" customFormat="1">
       <c r="A114" s="55"/>
       <c r="B114" s="55"/>
       <c r="C114" s="55"/>
       <c r="D114" s="56"/>
       <c r="E114" s="57"/>
     </row>
-    <row r="115" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" s="1" customFormat="1">
       <c r="A115" s="55"/>
       <c r="B115" s="55"/>
       <c r="C115" s="55"/>
       <c r="D115" s="56"/>
       <c r="E115" s="57"/>
     </row>
-    <row r="116" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" s="1" customFormat="1">
       <c r="A116" s="55"/>
       <c r="B116" s="55"/>
       <c r="C116" s="55"/>
       <c r="D116" s="56"/>
       <c r="E116" s="57"/>
     </row>
-    <row r="117" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" s="1" customFormat="1">
       <c r="A117" s="55"/>
       <c r="B117" s="55"/>
       <c r="C117" s="55"/>
       <c r="D117" s="56"/>
       <c r="E117" s="57"/>
     </row>
-    <row r="118" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" s="1" customFormat="1">
       <c r="A118" s="55"/>
       <c r="B118" s="55"/>
       <c r="C118" s="55"/>
       <c r="D118" s="56"/>
       <c r="E118" s="57"/>
     </row>
-    <row r="119" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" s="1" customFormat="1">
       <c r="A119" s="55"/>
       <c r="B119" s="55"/>
       <c r="C119" s="55"/>
       <c r="D119" s="56"/>
       <c r="E119" s="57"/>
     </row>
-    <row r="120" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" s="1" customFormat="1">
       <c r="A120" s="55"/>
       <c r="B120" s="55"/>
       <c r="C120" s="55"/>
       <c r="D120" s="56"/>
       <c r="E120" s="57"/>
     </row>
-    <row r="121" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" s="1" customFormat="1">
       <c r="A121" s="55"/>
       <c r="B121" s="55"/>
       <c r="C121" s="55"/>
       <c r="D121" s="56"/>
       <c r="E121" s="57"/>
     </row>
-    <row r="122" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" s="1" customFormat="1">
       <c r="A122" s="55"/>
       <c r="B122" s="55"/>
       <c r="C122" s="55"/>
       <c r="D122" s="56"/>
       <c r="E122" s="57"/>
     </row>
-    <row r="123" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" s="1" customFormat="1">
       <c r="A123" s="55"/>
       <c r="B123" s="55"/>
       <c r="C123" s="55"/>
       <c r="D123" s="56"/>
       <c r="E123" s="57"/>
     </row>
-    <row r="124" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" s="1" customFormat="1">
       <c r="A124" s="55"/>
       <c r="B124" s="55"/>
       <c r="C124" s="55"/>
       <c r="D124" s="56"/>
       <c r="E124" s="57"/>
     </row>
-    <row r="125" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" s="1" customFormat="1">
       <c r="A125" s="55"/>
       <c r="B125" s="55"/>
       <c r="C125" s="55"/>
       <c r="D125" s="56"/>
       <c r="E125" s="57"/>
     </row>
-    <row r="126" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" s="1" customFormat="1">
       <c r="A126" s="55"/>
       <c r="B126" s="55"/>
       <c r="C126" s="55"/>
       <c r="D126" s="56"/>
       <c r="E126" s="57"/>
     </row>
-    <row r="127" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" s="1" customFormat="1">
       <c r="A127" s="55"/>
       <c r="B127" s="55"/>
       <c r="C127" s="55"/>
       <c r="D127" s="56"/>
       <c r="E127" s="57"/>
     </row>
-    <row r="128" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" s="1" customFormat="1">
       <c r="A128" s="55"/>
       <c r="B128" s="55"/>
       <c r="C128" s="55"/>
       <c r="D128" s="56"/>
       <c r="E128" s="57"/>
     </row>
-    <row r="129" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" s="1" customFormat="1">
       <c r="A129" s="55"/>
       <c r="B129" s="55"/>
       <c r="C129" s="55"/>
       <c r="D129" s="56"/>
       <c r="E129" s="57"/>
     </row>
-    <row r="130" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" s="1" customFormat="1">
       <c r="A130" s="55"/>
       <c r="B130" s="55"/>
       <c r="C130" s="55"/>
       <c r="D130" s="56"/>
       <c r="E130" s="57"/>
     </row>
-    <row r="131" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" s="1" customFormat="1">
       <c r="A131" s="55"/>
       <c r="B131" s="55"/>
       <c r="C131" s="55"/>
       <c r="D131" s="56"/>
       <c r="E131" s="57"/>
     </row>
-    <row r="132" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" s="1" customFormat="1">
       <c r="A132" s="55"/>
       <c r="B132" s="55"/>
       <c r="C132" s="55"/>
       <c r="D132" s="56"/>
       <c r="E132" s="57"/>
     </row>
-    <row r="133" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" s="1" customFormat="1">
       <c r="A133" s="55"/>
       <c r="B133" s="55"/>
       <c r="C133" s="55"/>
       <c r="D133" s="56"/>
       <c r="E133" s="57"/>
     </row>
-    <row r="134" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" s="1" customFormat="1">
       <c r="A134" s="55"/>
       <c r="B134" s="55"/>
       <c r="C134" s="55"/>
       <c r="D134" s="56"/>
       <c r="E134" s="57"/>
     </row>
-    <row r="135" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" s="1" customFormat="1">
       <c r="A135" s="55"/>
       <c r="B135" s="55"/>
       <c r="C135" s="55"/>
       <c r="D135" s="56"/>
       <c r="E135" s="57"/>
     </row>
-    <row r="136" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" s="1" customFormat="1">
       <c r="A136" s="55"/>
       <c r="B136" s="55"/>
       <c r="C136" s="55"/>
       <c r="D136" s="56"/>
       <c r="E136" s="57"/>
     </row>
-    <row r="137" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" s="1" customFormat="1">
       <c r="A137" s="55"/>
       <c r="B137" s="55"/>
       <c r="C137" s="55"/>
       <c r="D137" s="56"/>
       <c r="E137" s="57"/>
     </row>
-    <row r="138" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" s="1" customFormat="1">
       <c r="A138" s="55"/>
       <c r="B138" s="55"/>
       <c r="C138" s="55"/>
       <c r="D138" s="56"/>
       <c r="E138" s="57"/>
     </row>
-    <row r="139" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" s="1" customFormat="1">
       <c r="A139" s="55"/>
       <c r="B139" s="55"/>
       <c r="C139" s="55"/>
       <c r="D139" s="56"/>
       <c r="E139" s="57"/>
     </row>
-    <row r="140" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" s="1" customFormat="1">
       <c r="A140" s="55"/>
       <c r="B140" s="55"/>
       <c r="C140" s="55"/>
       <c r="D140" s="56"/>
       <c r="E140" s="57"/>
     </row>
-    <row r="141" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" s="1" customFormat="1">
       <c r="A141" s="55"/>
       <c r="B141" s="55"/>
       <c r="C141" s="55"/>
       <c r="D141" s="56"/>
       <c r="E141" s="57"/>
     </row>
-    <row r="142" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" s="1" customFormat="1">
       <c r="A142" s="55"/>
       <c r="B142" s="55"/>
       <c r="C142" s="55"/>
       <c r="D142" s="56"/>
       <c r="E142" s="57"/>
     </row>
-    <row r="143" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" s="1" customFormat="1">
       <c r="A143" s="55"/>
       <c r="B143" s="55"/>
       <c r="C143" s="55"/>
       <c r="D143" s="56"/>
       <c r="E143" s="57"/>
     </row>
-    <row r="144" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" s="1" customFormat="1">
       <c r="A144" s="55"/>
       <c r="B144" s="55"/>
       <c r="C144" s="55"/>
       <c r="D144" s="56"/>
       <c r="E144" s="57"/>
     </row>
-    <row r="145" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" s="1" customFormat="1">
       <c r="A145" s="55"/>
       <c r="B145" s="55"/>
       <c r="C145" s="55"/>
       <c r="D145" s="56"/>
       <c r="E145" s="57"/>
     </row>
-    <row r="146" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" s="1" customFormat="1">
       <c r="A146" s="55"/>
       <c r="B146" s="55"/>
       <c r="C146" s="55"/>
       <c r="D146" s="56"/>
       <c r="E146" s="57"/>
     </row>
-    <row r="147" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" s="1" customFormat="1">
       <c r="A147" s="55"/>
       <c r="B147" s="55"/>
       <c r="C147" s="55"/>
       <c r="D147" s="56"/>
       <c r="E147" s="57"/>
     </row>
-    <row r="148" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" s="1" customFormat="1">
       <c r="A148" s="55"/>
       <c r="B148" s="55"/>
       <c r="C148" s="55"/>
       <c r="D148" s="56"/>
       <c r="E148" s="57"/>
     </row>
-    <row r="149" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" s="1" customFormat="1">
       <c r="A149" s="55"/>
       <c r="B149" s="55"/>
       <c r="C149" s="55"/>
       <c r="D149" s="56"/>
       <c r="E149" s="57"/>
     </row>
-    <row r="150" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" s="1" customFormat="1">
       <c r="A150" s="55"/>
       <c r="B150" s="55"/>
       <c r="C150" s="55"/>
       <c r="D150" s="56"/>
       <c r="E150" s="57"/>
     </row>
-    <row r="151" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" s="1" customFormat="1">
       <c r="A151" s="55"/>
       <c r="B151" s="55"/>
       <c r="C151" s="55"/>
       <c r="D151" s="56"/>
       <c r="E151" s="57"/>
     </row>
-    <row r="152" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" s="1" customFormat="1">
       <c r="A152" s="55"/>
       <c r="B152" s="55"/>
       <c r="C152" s="55"/>
       <c r="D152" s="56"/>
       <c r="E152" s="57"/>
     </row>
-    <row r="153" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" s="1" customFormat="1">
       <c r="A153" s="55"/>
       <c r="B153" s="55"/>
       <c r="C153" s="55"/>
       <c r="D153" s="56"/>
       <c r="E153" s="57"/>
     </row>
-    <row r="154" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" s="1" customFormat="1">
       <c r="A154" s="55"/>
       <c r="B154" s="55"/>
       <c r="C154" s="55"/>
       <c r="D154" s="56"/>
       <c r="E154" s="57"/>
     </row>
-    <row r="155" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" s="1" customFormat="1">
       <c r="A155" s="55"/>
       <c r="B155" s="55"/>
       <c r="C155" s="55"/>
       <c r="D155" s="56"/>
       <c r="E155" s="57"/>
     </row>
-    <row r="156" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" s="1" customFormat="1">
       <c r="A156" s="55"/>
       <c r="B156" s="55"/>
       <c r="C156" s="55"/>
       <c r="D156" s="56"/>
       <c r="E156" s="57"/>
     </row>
-    <row r="157" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" s="1" customFormat="1">
       <c r="A157" s="55"/>
       <c r="B157" s="55"/>
       <c r="C157" s="55"/>
       <c r="D157" s="56"/>
       <c r="E157" s="57"/>
     </row>
-    <row r="158" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" s="1" customFormat="1">
       <c r="A158" s="55"/>
       <c r="B158" s="55"/>
       <c r="C158" s="55"/>
       <c r="D158" s="56"/>
       <c r="E158" s="57"/>
     </row>
-    <row r="159" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" s="1" customFormat="1">
       <c r="A159" s="55"/>
       <c r="B159" s="55"/>
       <c r="C159" s="55"/>
       <c r="D159" s="56"/>
       <c r="E159" s="57"/>
     </row>
-    <row r="160" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" s="1" customFormat="1">
       <c r="A160" s="55"/>
       <c r="B160" s="55"/>
       <c r="C160" s="55"/>
       <c r="D160" s="56"/>
       <c r="E160" s="57"/>
     </row>
-    <row r="161" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" s="1" customFormat="1">
       <c r="A161" s="55"/>
       <c r="B161" s="55"/>
       <c r="C161" s="55"/>
       <c r="D161" s="56"/>
       <c r="E161" s="57"/>
     </row>
-    <row r="162" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" s="1" customFormat="1">
       <c r="A162" s="55"/>
       <c r="B162" s="55"/>
       <c r="C162" s="55"/>
       <c r="D162" s="56"/>
       <c r="E162" s="57"/>
     </row>
-    <row r="163" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" s="1" customFormat="1">
       <c r="A163" s="55"/>
       <c r="B163" s="55"/>
       <c r="C163" s="55"/>
       <c r="D163" s="56"/>
       <c r="E163" s="57"/>
     </row>
-    <row r="164" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" s="1" customFormat="1">
       <c r="A164" s="55"/>
       <c r="B164" s="55"/>
       <c r="C164" s="55"/>
       <c r="D164" s="56"/>
       <c r="E164" s="57"/>
     </row>
-    <row r="165" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" s="1" customFormat="1">
       <c r="A165" s="55"/>
       <c r="B165" s="55"/>
       <c r="C165" s="55"/>
       <c r="D165" s="56"/>
       <c r="E165" s="57"/>
     </row>
-    <row r="166" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" s="1" customFormat="1">
       <c r="A166" s="55"/>
       <c r="B166" s="55"/>
       <c r="C166" s="55"/>
       <c r="D166" s="56"/>
       <c r="E166" s="57"/>
     </row>
-    <row r="167" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" s="1" customFormat="1">
       <c r="A167" s="55"/>
       <c r="B167" s="55"/>
       <c r="C167" s="55"/>
       <c r="D167" s="56"/>
       <c r="E167" s="57"/>
     </row>
-    <row r="168" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" s="1" customFormat="1">
       <c r="A168" s="55"/>
       <c r="B168" s="55"/>
       <c r="C168" s="55"/>
       <c r="D168" s="56"/>
       <c r="E168" s="57"/>
     </row>
-    <row r="169" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" s="1" customFormat="1">
       <c r="A169" s="55"/>
       <c r="B169" s="55"/>
       <c r="C169" s="55"/>
       <c r="D169" s="56"/>
       <c r="E169" s="57"/>
     </row>
-    <row r="170" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" s="1" customFormat="1">
       <c r="A170" s="55"/>
       <c r="B170" s="55"/>
       <c r="C170" s="55"/>
       <c r="D170" s="56"/>
       <c r="E170" s="57"/>
     </row>
-    <row r="171" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" s="1" customFormat="1">
       <c r="A171" s="55"/>
       <c r="B171" s="55"/>
       <c r="C171" s="55"/>
       <c r="D171" s="56"/>
       <c r="E171" s="57"/>
     </row>
-    <row r="172" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" s="1" customFormat="1">
       <c r="A172" s="55"/>
       <c r="B172" s="55"/>
       <c r="C172" s="55"/>
       <c r="D172" s="56"/>
       <c r="E172" s="57"/>
     </row>
-    <row r="173" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" s="1" customFormat="1">
       <c r="A173" s="55"/>
       <c r="B173" s="55"/>
       <c r="C173" s="55"/>
       <c r="D173" s="56"/>
       <c r="E173" s="57"/>
     </row>
-    <row r="174" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" s="1" customFormat="1">
       <c r="A174" s="55"/>
       <c r="B174" s="55"/>
       <c r="C174" s="55"/>
       <c r="D174" s="56"/>
       <c r="E174" s="57"/>
     </row>
-    <row r="175" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" s="1" customFormat="1">
       <c r="A175" s="55"/>
       <c r="B175" s="55"/>
       <c r="C175" s="55"/>
       <c r="D175" s="56"/>
       <c r="E175" s="57"/>
     </row>
-    <row r="176" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" s="1" customFormat="1">
       <c r="A176" s="55"/>
       <c r="B176" s="55"/>
       <c r="C176" s="55"/>
       <c r="D176" s="56"/>
       <c r="E176" s="57"/>
     </row>
-    <row r="177" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" s="1" customFormat="1">
       <c r="A177" s="55"/>
       <c r="B177" s="55"/>
       <c r="C177" s="55"/>
       <c r="D177" s="56"/>
       <c r="E177" s="57"/>
     </row>
-    <row r="178" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" s="1" customFormat="1">
       <c r="A178" s="55"/>
       <c r="B178" s="55"/>
       <c r="C178" s="55"/>
       <c r="D178" s="56"/>
       <c r="E178" s="57"/>
     </row>
-    <row r="179" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" s="1" customFormat="1">
       <c r="A179" s="55"/>
       <c r="B179" s="55"/>
       <c r="C179" s="55"/>
       <c r="D179" s="56"/>
       <c r="E179" s="57"/>
     </row>
-    <row r="180" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" s="1" customFormat="1">
       <c r="A180" s="55"/>
       <c r="B180" s="55"/>
       <c r="C180" s="55"/>
       <c r="D180" s="56"/>
       <c r="E180" s="57"/>
     </row>
-    <row r="181" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" s="1" customFormat="1">
       <c r="A181" s="55"/>
       <c r="B181" s="55"/>
       <c r="C181" s="55"/>
       <c r="D181" s="56"/>
       <c r="E181" s="57"/>
     </row>
-    <row r="182" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" s="1" customFormat="1">
       <c r="A182" s="55"/>
       <c r="B182" s="55"/>
       <c r="C182" s="55"/>
       <c r="D182" s="56"/>
       <c r="E182" s="57"/>
     </row>
-    <row r="183" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" s="1" customFormat="1">
       <c r="A183" s="55"/>
       <c r="B183" s="55"/>
       <c r="C183" s="55"/>
       <c r="D183" s="56"/>
       <c r="E183" s="57"/>
     </row>
-    <row r="184" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" s="1" customFormat="1">
       <c r="A184" s="55"/>
       <c r="B184" s="55"/>
       <c r="C184" s="55"/>
       <c r="D184" s="56"/>
       <c r="E184" s="57"/>
     </row>
-    <row r="185" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" s="1" customFormat="1">
       <c r="A185" s="55"/>
       <c r="B185" s="55"/>
       <c r="C185" s="55"/>
       <c r="D185" s="56"/>
       <c r="E185" s="57"/>
     </row>
-    <row r="186" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" s="1" customFormat="1">
       <c r="A186" s="55"/>
       <c r="B186" s="55"/>
       <c r="C186" s="55"/>
       <c r="D186" s="56"/>
       <c r="E186" s="57"/>
     </row>
-    <row r="187" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" s="1" customFormat="1">
       <c r="A187" s="55"/>
       <c r="B187" s="55"/>
       <c r="C187" s="55"/>
       <c r="D187" s="56"/>
       <c r="E187" s="57"/>
     </row>
-    <row r="188" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" s="1" customFormat="1">
       <c r="A188" s="55"/>
       <c r="B188" s="55"/>
       <c r="C188" s="55"/>
       <c r="D188" s="56"/>
       <c r="E188" s="57"/>
     </row>
-    <row r="189" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" s="1" customFormat="1">
       <c r="A189" s="55"/>
       <c r="B189" s="55"/>
       <c r="C189" s="55"/>
       <c r="D189" s="56"/>
       <c r="E189" s="57"/>
     </row>
-    <row r="190" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" s="1" customFormat="1">
       <c r="A190" s="55"/>
       <c r="B190" s="55"/>
       <c r="C190" s="55"/>
       <c r="D190" s="56"/>
       <c r="E190" s="57"/>
     </row>
-    <row r="191" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" s="1" customFormat="1">
       <c r="A191" s="55"/>
       <c r="B191" s="55"/>
       <c r="C191" s="55"/>
       <c r="D191" s="56"/>
       <c r="E191" s="57"/>
     </row>
-    <row r="192" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" s="1" customFormat="1">
       <c r="A192" s="55"/>
       <c r="B192" s="55"/>
       <c r="C192" s="55"/>
       <c r="D192" s="56"/>
       <c r="E192" s="57"/>
     </row>
-    <row r="193" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" s="1" customFormat="1">
       <c r="A193" s="55"/>
       <c r="B193" s="55"/>
       <c r="C193" s="55"/>
       <c r="D193" s="56"/>
       <c r="E193" s="57"/>
     </row>
-    <row r="194" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" s="1" customFormat="1">
       <c r="A194" s="55"/>
       <c r="B194" s="55"/>
       <c r="C194" s="55"/>
       <c r="D194" s="56"/>
       <c r="E194" s="58"/>
     </row>
-    <row r="195" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" s="1" customFormat="1">
       <c r="A195" s="55"/>
       <c r="B195" s="55"/>
       <c r="C195" s="55"/>
       <c r="D195" s="56"/>
       <c r="E195" s="58"/>
     </row>
-    <row r="196" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" s="1" customFormat="1">
       <c r="A196" s="55"/>
       <c r="B196" s="55"/>
       <c r="C196" s="55"/>
       <c r="D196" s="56"/>
       <c r="E196" s="58"/>
     </row>
-    <row r="197" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" s="1" customFormat="1">
       <c r="A197" s="55"/>
       <c r="B197" s="55"/>
       <c r="C197" s="55"/>
       <c r="D197" s="56"/>
       <c r="E197" s="58"/>
     </row>
-    <row r="198" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" s="1" customFormat="1">
       <c r="A198" s="55"/>
       <c r="B198" s="55"/>
       <c r="C198" s="55"/>
       <c r="D198" s="56"/>
       <c r="E198" s="58"/>
     </row>
-    <row r="199" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" s="1" customFormat="1">
       <c r="A199" s="55"/>
       <c r="B199" s="55"/>
       <c r="C199" s="55"/>
       <c r="D199" s="56"/>
       <c r="E199" s="58"/>
     </row>
-    <row r="200" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" s="1" customFormat="1">
       <c r="A200" s="55"/>
       <c r="B200" s="55"/>
       <c r="C200" s="55"/>
       <c r="D200" s="56"/>
       <c r="E200" s="58"/>
     </row>
-    <row r="201" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" s="1" customFormat="1">
       <c r="A201" s="55"/>
       <c r="B201" s="55"/>
       <c r="C201" s="55"/>
       <c r="D201" s="56"/>
       <c r="E201" s="58"/>
     </row>
-    <row r="202" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" s="1" customFormat="1">
       <c r="A202" s="55"/>
       <c r="B202" s="55"/>
       <c r="C202" s="55"/>
       <c r="D202" s="56"/>
       <c r="E202" s="58"/>
     </row>
-    <row r="203" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" s="1" customFormat="1">
       <c r="A203" s="55"/>
       <c r="B203" s="55"/>
       <c r="C203" s="55"/>
       <c r="D203" s="56"/>
       <c r="E203" s="58"/>
     </row>
-    <row r="204" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" s="1" customFormat="1">
       <c r="A204" s="55"/>
       <c r="B204" s="55"/>
       <c r="C204" s="55"/>
       <c r="D204" s="56"/>
       <c r="E204" s="58"/>
     </row>
-    <row r="205" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" s="1" customFormat="1">
       <c r="A205" s="55"/>
       <c r="B205" s="55"/>
       <c r="C205" s="55"/>
       <c r="D205" s="56"/>
       <c r="E205" s="58"/>
     </row>
-    <row r="206" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" s="1" customFormat="1">
       <c r="A206" s="55"/>
       <c r="B206" s="55"/>
       <c r="C206" s="55"/>
       <c r="D206" s="56"/>
       <c r="E206" s="58"/>
     </row>
-    <row r="207" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" s="1" customFormat="1">
       <c r="A207" s="55"/>
       <c r="B207" s="55"/>
       <c r="C207" s="55"/>
       <c r="D207" s="56"/>
       <c r="E207" s="58"/>
     </row>
-    <row r="208" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" s="1" customFormat="1">
       <c r="A208" s="55"/>
       <c r="B208" s="55"/>
       <c r="C208" s="55"/>
       <c r="D208" s="56"/>
       <c r="E208" s="58"/>
     </row>
-    <row r="209" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" s="1" customFormat="1">
       <c r="A209" s="55"/>
       <c r="B209" s="55"/>
       <c r="C209" s="55"/>
       <c r="D209" s="56"/>
       <c r="E209" s="58"/>
     </row>
-    <row r="210" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" s="1" customFormat="1">
       <c r="A210" s="55"/>
       <c r="B210" s="55"/>
       <c r="C210" s="55"/>
       <c r="D210" s="56"/>
       <c r="E210" s="58"/>
     </row>
-    <row r="211" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" s="1" customFormat="1">
       <c r="A211" s="55"/>
       <c r="B211" s="55"/>
       <c r="C211" s="55"/>
       <c r="D211" s="56"/>
       <c r="E211" s="58"/>
     </row>
-    <row r="212" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" s="1" customFormat="1">
       <c r="A212" s="55"/>
       <c r="B212" s="55"/>
       <c r="C212" s="55"/>
       <c r="D212" s="56"/>
       <c r="E212" s="58"/>
     </row>
-    <row r="213" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" s="1" customFormat="1">
       <c r="A213" s="55"/>
       <c r="B213" s="55"/>
       <c r="C213" s="55"/>
       <c r="D213" s="56"/>
       <c r="E213" s="58"/>
     </row>
-    <row r="214" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" s="1" customFormat="1">
       <c r="A214" s="55"/>
       <c r="B214" s="55"/>
       <c r="C214" s="55"/>
       <c r="D214" s="56"/>
       <c r="E214" s="58"/>
     </row>
-    <row r="215" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" s="1" customFormat="1">
       <c r="A215" s="55"/>
       <c r="B215" s="55"/>
       <c r="C215" s="55"/>
       <c r="D215" s="56"/>
       <c r="E215" s="58"/>
     </row>
-    <row r="216" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" s="1" customFormat="1">
       <c r="A216" s="55"/>
       <c r="B216" s="55"/>
       <c r="C216" s="55"/>
       <c r="D216" s="56"/>
       <c r="E216" s="58"/>
     </row>
-    <row r="217" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" s="1" customFormat="1">
       <c r="A217" s="55"/>
       <c r="B217" s="55"/>
       <c r="C217" s="55"/>
       <c r="D217" s="56"/>
       <c r="E217" s="58"/>
     </row>
-    <row r="218" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" s="1" customFormat="1">
       <c r="A218" s="55"/>
       <c r="B218" s="55"/>
       <c r="C218" s="55"/>
       <c r="D218" s="56"/>
       <c r="E218" s="58"/>
     </row>
-    <row r="219" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" s="1" customFormat="1">
       <c r="A219" s="55"/>
       <c r="B219" s="55"/>
       <c r="C219" s="55"/>
       <c r="D219" s="56"/>
       <c r="E219" s="58"/>
     </row>
-    <row r="220" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" s="1" customFormat="1">
       <c r="A220" s="55"/>
       <c r="B220" s="55"/>
       <c r="C220" s="55"/>
       <c r="D220" s="56"/>
       <c r="E220" s="58"/>
     </row>
-    <row r="221" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" s="1" customFormat="1">
       <c r="A221" s="55"/>
       <c r="B221" s="55"/>
       <c r="C221" s="55"/>
       <c r="D221" s="56"/>
       <c r="E221" s="58"/>
     </row>
-    <row r="222" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" s="1" customFormat="1">
       <c r="A222" s="55"/>
       <c r="B222" s="55"/>
       <c r="C222" s="55"/>
       <c r="D222" s="56"/>
       <c r="E222" s="58"/>
     </row>
-    <row r="223" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" s="1" customFormat="1">
       <c r="A223" s="55"/>
       <c r="B223" s="55"/>
       <c r="C223" s="55"/>
       <c r="D223" s="56"/>
       <c r="E223" s="58"/>
     </row>
-    <row r="224" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" s="1" customFormat="1">
       <c r="A224" s="55"/>
       <c r="B224" s="55"/>
       <c r="C224" s="55"/>
       <c r="D224" s="56"/>
       <c r="E224" s="58"/>
     </row>
-    <row r="225" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" s="1" customFormat="1">
       <c r="A225" s="55"/>
       <c r="B225" s="55"/>
       <c r="C225" s="55"/>
       <c r="D225" s="56"/>
       <c r="E225" s="58"/>
     </row>
-    <row r="226" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" s="1" customFormat="1">
       <c r="A226" s="55"/>
       <c r="B226" s="55"/>
       <c r="C226" s="55"/>
       <c r="D226" s="56"/>
       <c r="E226" s="58"/>
     </row>
-    <row r="227" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" s="1" customFormat="1">
       <c r="A227" s="55"/>
       <c r="B227" s="55"/>
       <c r="C227" s="55"/>
       <c r="D227" s="56"/>
       <c r="E227" s="58"/>
     </row>
-    <row r="228" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" s="1" customFormat="1">
       <c r="A228" s="55"/>
       <c r="B228" s="55"/>
       <c r="C228" s="55"/>
       <c r="D228" s="56"/>
       <c r="E228" s="58"/>
     </row>
-    <row r="229" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" s="1" customFormat="1">
       <c r="A229" s="55"/>
       <c r="B229" s="55"/>
       <c r="C229" s="55"/>
       <c r="D229" s="56"/>
       <c r="E229" s="58"/>
     </row>
-    <row r="230" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" s="1" customFormat="1">
       <c r="A230" s="55"/>
       <c r="B230" s="55"/>
       <c r="C230" s="55"/>
       <c r="D230" s="56"/>
       <c r="E230" s="58"/>
     </row>
-    <row r="231" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" s="1" customFormat="1">
       <c r="A231" s="55"/>
       <c r="B231" s="55"/>
       <c r="C231" s="55"/>
       <c r="D231" s="56"/>
       <c r="E231" s="58"/>
     </row>
-    <row r="232" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" s="1" customFormat="1">
       <c r="A232" s="55"/>
       <c r="B232" s="55"/>
       <c r="C232" s="55"/>
       <c r="D232" s="56"/>
       <c r="E232" s="58"/>
     </row>
-    <row r="233" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" s="1" customFormat="1">
       <c r="A233" s="55"/>
       <c r="B233" s="55"/>
       <c r="C233" s="55"/>
       <c r="D233" s="56"/>
       <c r="E233" s="58"/>
     </row>
-    <row r="234" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" s="1" customFormat="1">
       <c r="A234" s="55"/>
       <c r="B234" s="55"/>
       <c r="C234" s="55"/>
       <c r="D234" s="56"/>
       <c r="E234" s="58"/>
     </row>
-    <row r="235" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" s="1" customFormat="1">
       <c r="A235" s="55"/>
       <c r="B235" s="55"/>
       <c r="C235" s="55"/>
       <c r="D235" s="56"/>
       <c r="E235" s="58"/>
     </row>
-    <row r="236" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" s="1" customFormat="1">
       <c r="A236" s="55"/>
       <c r="B236" s="55"/>
       <c r="C236" s="55"/>
       <c r="D236" s="56"/>
       <c r="E236" s="58"/>
     </row>
-    <row r="237" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" s="1" customFormat="1">
       <c r="A237" s="55"/>
       <c r="B237" s="55"/>
       <c r="C237" s="55"/>
       <c r="D237" s="56"/>
       <c r="E237" s="58"/>
     </row>
-    <row r="238" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" s="1" customFormat="1">
       <c r="A238" s="55"/>
       <c r="B238" s="55"/>
       <c r="C238" s="55"/>

</xml_diff>

<commit_message>
Allowed Driver Station to display the USB Cameras and wrote code to limit the USB and Axis Camera's FPS's. The Axis Camera's FPS is currently being set in firmware, but is still too high on the Driver's Station.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2017.xlsx
+++ b/Kilroy Equipment List 2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14670" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$102</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -209,6 +210,78 @@
   </si>
   <si>
     <t>12, 13</t>
+  </si>
+  <si>
+    <t>Left Operator 8</t>
+  </si>
+  <si>
+    <t>Axis Camera</t>
+  </si>
+  <si>
+    <t>axisCamera</t>
+  </si>
+  <si>
+    <t>10.3.39.11</t>
+  </si>
+  <si>
+    <t>USB Camera 0</t>
+  </si>
+  <si>
+    <t>cam0</t>
+  </si>
+  <si>
+    <t>cam1</t>
+  </si>
+  <si>
+    <t>USB Camera 1</t>
+  </si>
+  <si>
+    <t>Right Front Motor Controller</t>
+  </si>
+  <si>
+    <t>Left Front Motor Controller</t>
+  </si>
+  <si>
+    <t>leftFrontMotor</t>
+  </si>
+  <si>
+    <t>PWM 1</t>
+  </si>
+  <si>
+    <t>rightFrontMotor</t>
+  </si>
+  <si>
+    <t>PWM 4</t>
+  </si>
+  <si>
+    <t>pdp</t>
+  </si>
+  <si>
+    <t>Power Distribution Board/Panel</t>
+  </si>
+  <si>
+    <t>Ring Light Relay</t>
+  </si>
+  <si>
+    <t>ringlightRelay</t>
+  </si>
+  <si>
+    <t>Set Rotation Value</t>
+  </si>
+  <si>
+    <t>Right Driver Trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take Single Picture </t>
+  </si>
+  <si>
+    <t>Stop Aligning/ set isAligning to False</t>
+  </si>
+  <si>
+    <t>Left Operator 7</t>
+  </si>
+  <si>
+    <t>Start Aligning/ set isAligning to True</t>
   </si>
 </sst>
 </file>
@@ -947,8 +1020,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <pane ySplit="2" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1011,7 +1084,7 @@
         <v>37</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
@@ -1030,16 +1103,28 @@
     <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
+      <c r="C6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="34" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
+      <c r="C7" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="33"/>
@@ -1357,9 +1442,15 @@
       <c r="B44" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="46"/>
+      <c r="C44" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1">
       <c r="A45" s="40"/>
@@ -1501,9 +1592,15 @@
     <row r="62" spans="1:8" s="1" customFormat="1">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
+      <c r="C62" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1">
       <c r="A63" s="4"/>
@@ -1611,30 +1708,46 @@
     <row r="72" spans="1:8" s="1" customFormat="1">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
-      <c r="C72" s="23"/>
+      <c r="C72" s="23" t="s">
+        <v>82</v>
+      </c>
       <c r="D72" s="26"/>
-      <c r="E72" s="25"/>
+      <c r="E72" s="25" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="73" spans="1:8" s="35" customFormat="1">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="28"/>
+      <c r="C73" s="28" t="s">
+        <v>85</v>
+      </c>
       <c r="D73" s="31"/>
-      <c r="E73" s="32"/>
+      <c r="E73" s="32" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1">
       <c r="A74" s="47"/>
       <c r="B74" s="47"/>
-      <c r="C74" s="22"/>
+      <c r="C74" s="22" t="s">
+        <v>87</v>
+      </c>
       <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
+      <c r="E74" s="22" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="32"/>
+      <c r="C75" s="32" t="s">
+        <v>84</v>
+      </c>
       <c r="D75" s="31"/>
-      <c r="E75" s="32"/>
+      <c r="E75" s="32" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">
       <c r="A76" s="10"/>
@@ -1923,23 +2036,41 @@
     <row r="109" spans="1:6" s="1" customFormat="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="32"/>
+      <c r="C109" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D109" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E109" s="32" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="110" spans="1:6" s="1" customFormat="1">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
-      <c r="C110" s="22"/>
-      <c r="D110" s="44"/>
-      <c r="E110" s="22"/>
+      <c r="C110" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D110" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E110" s="22" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="111" spans="1:6" s="1" customFormat="1">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="28"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="32"/>
+      <c r="C111" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D111" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E111" s="32" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1">
       <c r="A112" s="13"/>

</xml_diff>